<commit_message>
Fix tests and improve how updating of patients is handled and fixes from review
</commit_message>
<xml_diff>
--- a/tests/data/data.xlsx
+++ b/tests/data/data.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t xml:space="preserve">PV 28 Září 2019</t>
   </si>
@@ -118,117 +118,6 @@
       <t xml:space="preserve"> DQ6, DQ5</t>
     </r>
   </si>
-  <si>
-    <t xml:space="preserve">P-3D</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DR13 DR53 DR52 DQ9 DQ6</t>
-  </si>
-  <si>
-    <t xml:space="preserve">P-3R</t>
-  </si>
-  <si>
-    <t xml:space="preserve">A2 B7 B8 DR17 DR4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">B67 B76 B54 B46 B56 B42 B58 B45 B78 B49 B50 B18 B35 B72 B71 B44 B62 A24 B57 Cw9 B27 B77 B75 B53 B13 B59</t>
-  </si>
-  <si>
-    <t xml:space="preserve">A25 A3 A66 A26 A34 A43 A11 A31 A80 A32 A74 B55 A33 A68 A29 A1 A69 A30 A36 B63 B67 B76 B54 B46 B56 B42</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0, A, B, AB</t>
-  </si>
-  <si>
-    <t xml:space="preserve">P-4D</t>
-  </si>
-  <si>
-    <t xml:space="preserve">B</t>
-  </si>
-  <si>
-    <t xml:space="preserve">B46 DR9 DR15 DR53 DR51</t>
-  </si>
-  <si>
-    <t xml:space="preserve">P-4R</t>
-  </si>
-  <si>
-    <t xml:space="preserve">A2 A11 B46 DR9</t>
-  </si>
-  <si>
-    <t xml:space="preserve">B41 B60 B48 B7 B42 B61 A1 B81 B8 B62 B76 B67 B71 B73 B27 B50 B51 B39 B49 B52 B18 B45 B</t>
-  </si>
-  <si>
-    <t xml:space="preserve">B41 B60 B48 B7 B42 B61 A1 B81 B8 B62 B76 B67 B71 B73 B27 B50 B51 B39 B49 B52 B18 B45 B44 B72 B13 B77 B35 B55</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0,A, B, AB</t>
-  </si>
-  <si>
-    <t xml:space="preserve">P-5D</t>
-  </si>
-  <si>
-    <t xml:space="preserve">A2 B35 B44 DR4 DR15 DR53</t>
-  </si>
-  <si>
-    <t xml:space="preserve">P-5R</t>
-  </si>
-  <si>
-    <t xml:space="preserve">A2 A26 B27 B62 DR1 DR8</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="238"/>
-      </rPr>
-      <t xml:space="preserve">B65, B67, </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="238"/>
-      </rPr>
-      <t xml:space="preserve">B77</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="238"/>
-      </rPr>
-      <t xml:space="preserve">, Cw5, DR53, DR7, DQ2, DQ7, DQ9, DR52, DQ4, DR12, DR9, DQ8, DR10</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <color rgb="FFFFC000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="238"/>
-      </rPr>
-      <t xml:space="preserve">A2</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="238"/>
-      </rPr>
-      <t xml:space="preserve">, A3, A24, A29, A30, A31, A33, A34</t>
-    </r>
-  </si>
 </sst>
 </file>
 
@@ -237,7 +126,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="12">
+  <fonts count="11">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -261,12 +150,6 @@
       <family val="0"/>
     </font>
     <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <charset val="238"/>
-    </font>
-    <font>
       <sz val="14"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
@@ -288,6 +171,12 @@
       <charset val="238"/>
     </font>
     <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="238"/>
+    </font>
+    <font>
       <sz val="9"/>
       <name val="Arial"/>
       <family val="2"/>
@@ -303,13 +192,6 @@
     <font>
       <sz val="9"/>
       <color rgb="FFFF0000"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <charset val="238"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color rgb="FFFFC000"/>
       <name val="Arial"/>
       <family val="2"/>
       <charset val="238"/>
@@ -394,17 +276,17 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="14">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -412,39 +294,39 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="5" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="4" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="5" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="4" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="5" borderId="1" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="5" borderId="1" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -452,11 +334,7 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -468,7 +346,7 @@
     <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
     <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
     <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
-    <cellStyle name="Normální 13" xfId="20" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Excel Built-in Explanatory Text" xfId="20" builtinId="53" customBuiltin="true"/>
   </cellStyles>
   <colors>
     <indexedColors>
@@ -541,7 +419,7 @@
   <dimension ref="A1:I1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A2" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G4" activeCellId="0" sqref="G4"/>
+      <selection pane="topLeft" activeCell="F14" activeCellId="0" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -621,93 +499,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="22.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="B4" s="9" t="n">
-        <v>0</v>
-      </c>
-      <c r="C4" s="10" t="s">
-        <v>18</v>
-      </c>
-      <c r="D4" s="11" t="s">
-        <v>19</v>
-      </c>
-      <c r="E4" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="F4" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="G4" s="12" t="s">
-        <v>21</v>
-      </c>
-      <c r="H4" s="12" t="s">
-        <v>22</v>
-      </c>
-      <c r="I4" s="13" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="22.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="B5" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="C5" s="10" t="s">
-        <v>26</v>
-      </c>
-      <c r="D5" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="E5" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="F5" s="10" t="s">
-        <v>28</v>
-      </c>
-      <c r="G5" s="12" t="s">
-        <v>29</v>
-      </c>
-      <c r="H5" s="12" t="s">
-        <v>30</v>
-      </c>
-      <c r="I5" s="13" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="22.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="8" t="s">
-        <v>32</v>
-      </c>
-      <c r="B6" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="C6" s="10" t="s">
-        <v>33</v>
-      </c>
-      <c r="D6" s="11" t="s">
-        <v>34</v>
-      </c>
-      <c r="E6" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="F6" s="10" t="s">
-        <v>35</v>
-      </c>
-      <c r="G6" s="12" t="s">
-        <v>36</v>
-      </c>
-      <c r="H6" s="14" t="s">
-        <v>37</v>
-      </c>
-      <c r="I6" s="13" t="s">
-        <v>23</v>
-      </c>
-    </row>
+    <row r="1048540" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048541" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048542" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048543" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048544" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048545" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>

</xml_diff>

<commit_message>
Fix small bugs, add tests
</commit_message>
<xml_diff>
--- a/tests/data/data.xlsx
+++ b/tests/data/data.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="21">
   <si>
     <t xml:space="preserve">PV 28 Září 2019</t>
   </si>
@@ -64,38 +64,10 @@
     <t xml:space="preserve">P11</t>
   </si>
   <si>
-    <t xml:space="preserve">A3 A26 B8 B38 DR17 DR4 </t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="238"/>
-      </rPr>
-      <t xml:space="preserve">B7, </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="238"/>
-      </rPr>
-      <t xml:space="preserve">B81, B27,</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="238"/>
-      </rPr>
-      <t xml:space="preserve"> DQ6, DQ5, DQ4, DR15, DR51</t>
-    </r>
+    <t xml:space="preserve">A3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A2</t>
   </si>
   <si>
     <r>
@@ -118,6 +90,18 @@
       <t xml:space="preserve"> DQ6, DQ5</t>
     </r>
   </si>
+  <si>
+    <t xml:space="preserve">A, 0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">P22</t>
+  </si>
+  <si>
+    <t xml:space="preserve">P12</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A11</t>
+  </si>
 </sst>
 </file>
 
@@ -126,7 +110,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="11">
+  <fonts count="10">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -185,13 +169,6 @@
     <font>
       <sz val="9"/>
       <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <charset val="238"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color rgb="FFFF0000"/>
       <name val="Arial"/>
       <family val="2"/>
       <charset val="238"/>
@@ -419,7 +396,7 @@
   <dimension ref="A1:I1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
+      <selection pane="topLeft" activeCell="G4" activeCellId="0" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -495,7 +472,36 @@
       <c r="H3" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="I3" s="13" t="n">
+      <c r="I3" s="13" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="B4" s="9" t="n">
+        <v>0</v>
+      </c>
+      <c r="C4" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="D4" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="E4" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="F4" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="G4" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="H4" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="I4" s="13" t="n">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
bugfix: failing tests due to forgotten update of the xlxs file when logic became more strict and allowed only truly valid patients
</commit_message>
<xml_diff>
--- a/tests/data/data.xlsx
+++ b/tests/data/data.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="23">
   <si>
     <t xml:space="preserve">PV 28 Září 2019</t>
   </si>
@@ -58,13 +58,30 @@
     <t xml:space="preserve">A</t>
   </si>
   <si>
-    <t xml:space="preserve">A11 </t>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="238"/>
+      </rPr>
+      <t xml:space="preserve">A11,</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">B8,DR11</t>
+    </r>
   </si>
   <si>
     <t xml:space="preserve">P11</t>
   </si>
   <si>
-    <t xml:space="preserve">A3</t>
+    <t xml:space="preserve">A3,B7,DR11</t>
   </si>
   <si>
     <t xml:space="preserve">A2</t>
@@ -97,7 +114,47 @@
     <t xml:space="preserve">P22</t>
   </si>
   <si>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="238"/>
+      </rPr>
+      <t xml:space="preserve">A2,</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">B8,DR11</t>
+    </r>
+  </si>
+  <si>
     <t xml:space="preserve">P12</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="238"/>
+      </rPr>
+      <t xml:space="preserve">A3,</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">B7,DR11</t>
+    </r>
   </si>
   <si>
     <t xml:space="preserve">A11</t>
@@ -110,7 +167,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="10">
+  <fonts count="11">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -165,6 +222,12 @@
       <name val="Arial"/>
       <family val="2"/>
       <charset val="238"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="9"/>
@@ -307,7 +370,7 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -317,13 +380,13 @@
     </xf>
   </cellXfs>
   <cellStyles count="7">
-    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
-    <cellStyle name="Excel Built-in Explanatory Text" xfId="20" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Comma" xfId="15" builtinId="3"/>
+    <cellStyle name="Comma [0]" xfId="16" builtinId="6"/>
+    <cellStyle name="Currency" xfId="17" builtinId="4"/>
+    <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
+    <cellStyle name="Percent" xfId="19" builtinId="5"/>
+    <cellStyle name="Excel Built-in Explanatory Text" xfId="20"/>
   </cellStyles>
   <colors>
     <indexedColors>
@@ -396,20 +459,17 @@
   <dimension ref="A1:I1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G4" activeCellId="0" sqref="G4"/>
+      <selection pane="topLeft" activeCell="C4" activeCellId="0" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.6875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="8.67"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="31.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="10.99"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="8.67"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="23.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="54.3"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="62.98"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="11.3"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="10" style="0" width="8.67"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="31.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -484,19 +544,19 @@
         <v>0</v>
       </c>
       <c r="C4" s="10" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="D4" s="11" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E4" s="9" t="s">
         <v>11</v>
       </c>
       <c r="F4" s="10" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="G4" s="10" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="H4" s="12" t="s">
         <v>16</v>

</xml_diff>